<commit_message>
fixes errors in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_redd_metadata.xlsx
+++ b/data-raw/metadata/yuba_redd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60B015A-11E6-BD4E-BC0A-31092ED84A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22375BF2-30C3-EB42-B45C-C43C6353274A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-9480" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Water depth measured at sampling</t>
   </si>
   <si>
-    <t>Species associated with the sampled redd</t>
-  </si>
-  <si>
     <t>feetPerSecond</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
   </si>
   <si>
     <t>degree</t>
-  </si>
-  <si>
-    <t>Number of fish observed on the redd at time of sampling Levels = c("chinook", "unknown", "steelhead")</t>
   </si>
   <si>
     <t>redd</t>
@@ -173,6 +167,12 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of fish observed on the redd at time of sampling </t>
+  </si>
+  <si>
+    <t>Species associated with the sampled redd. Levels = c("chinook", "unknown", "steelhead")</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -574,7 +574,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>17</v>
@@ -584,14 +584,14 @@
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="J2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -618,7 +618,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>16</v>
@@ -627,10 +627,10 @@
         <v>15</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="5"/>
@@ -666,7 +666,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>16</v>
@@ -675,10 +675,10 @@
         <v>15</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="5"/>
@@ -714,7 +714,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>14</v>
@@ -752,7 +752,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>16</v>
@@ -761,10 +761,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="5"/>
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>16</v>
@@ -809,10 +809,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="5"/>
@@ -842,13 +842,13 @@
         <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>14</v>
@@ -880,13 +880,13 @@
         <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>16</v>
@@ -895,10 +895,10 @@
         <v>15</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>

</xml_diff>

<commit_message>
updates metadata for tables and re-writes xml and validates
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_redd_metadata.xlsx
+++ b/data-raw/metadata/yuba_redd_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-yuba-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22375BF2-30C3-EB42-B45C-C43C6353274A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0340DC45-4C1F-1B41-8E3D-8D91241E8D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Species associated with the sampled redd. Levels = c("chinook", "unknown", "steelhead")</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Run designation of fish associated with redd. Levels = "not recorded"</t>
   </si>
 </sst>
 </file>
@@ -485,11 +491,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -705,28 +711,38 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="16">
+        <v>2.2066669999999999</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -743,38 +759,28 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="6"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="14">
-        <v>0</v>
-      </c>
-      <c r="M6" s="16">
-        <v>2.2066669999999999</v>
-      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -791,38 +797,28 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>36</v>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="6"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="14">
-        <v>0</v>
-      </c>
-      <c r="M7" s="14">
-        <v>1.7</v>
-      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -839,28 +835,38 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>48</v>
+      <c r="B8" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="L8" s="14">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14">
+        <v>1.7</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -877,38 +883,28 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
-        <v>8</v>
-      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -924,19 +920,39 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>8</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -963,8 +979,8 @@
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1047,8 +1063,8 @@
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="5"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1076,7 +1092,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="12"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1131,7 +1147,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="10"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="5"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1149,18 +1165,18 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="5"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1259,8 +1275,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1286,9 +1303,8 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
@@ -1456,34 +1472,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1515,29 +1531,39 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1556,16 +1582,6 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1696,6 +1712,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1723,7 +1740,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1751,6 +1767,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1778,7 +1795,6 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2730,7 +2746,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28657,18 +28673,46 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
+    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="3"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="3"/>
+      <c r="M1001" s="3"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C9:C32 C1:C8" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E9:E32 E1:E8" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F9:F32 F1:F8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H9:H32 H1:H8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>